<commit_message>
captions and other graphical updates
</commit_message>
<xml_diff>
--- a/ges_health_study_app/dictionary_english.xlsx
+++ b/ges_health_study_app/dictionary_english.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65328A0-0D22-1A42-8CBB-819361E4927C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA35873B-AD0F-084A-8B7A-4DD8F7A15F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37300" yWindow="500" windowWidth="16240" windowHeight="19840" xr2:uid="{FBC012AF-A400-554A-B28E-7E1CB6FB8950}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{FBC012AF-A400-554A-B28E-7E1CB6FB8950}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -764,10 +764,10 @@
     <t>lbw_pct</t>
   </si>
   <si>
-    <t>Per 10,000</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chronic kidney disease among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t>Cases per 10,000</t>
   </si>
 </sst>
 </file>
@@ -816,13 +816,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1159,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEABDE7F-51DA-E349-ABBB-2A88FDA51C20}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1839,7 +1838,7 @@
       <c r="H19" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" t="s">
         <v>130</v>
       </c>
       <c r="J19" t="s">
@@ -1877,7 +1876,7 @@
       <c r="H20" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" t="s">
         <v>128</v>
       </c>
       <c r="J20" t="s">
@@ -1915,7 +1914,7 @@
       <c r="H21" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" t="s">
         <v>130</v>
       </c>
       <c r="J21" t="s">
@@ -1953,7 +1952,7 @@
       <c r="H22" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" t="s">
         <v>128</v>
       </c>
       <c r="J22" t="s">
@@ -1991,7 +1990,7 @@
       <c r="H23" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" t="s">
         <v>128</v>
       </c>
       <c r="J23" t="s">
@@ -2029,7 +2028,7 @@
       <c r="H24" t="s">
         <v>39</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" t="s">
         <v>129</v>
       </c>
       <c r="J24" t="s">
@@ -2064,7 +2063,7 @@
       <c r="H25" t="s">
         <v>39</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" t="s">
         <v>135</v>
       </c>
       <c r="J25" t="s">
@@ -2100,10 +2099,10 @@
       <c r="H26" t="s">
         <v>39</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J26" s="3" t="s">
+      <c r="I26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" t="s">
         <v>41</v>
       </c>
       <c r="K26" t="s">
@@ -2136,10 +2135,10 @@
       <c r="H27" t="s">
         <v>39</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J27" s="3" t="s">
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s">
         <v>41</v>
       </c>
       <c r="K27" t="s">
@@ -2172,10 +2171,10 @@
       <c r="H28" t="s">
         <v>39</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="3" t="s">
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" t="s">
         <v>41</v>
       </c>
       <c r="K28" t="s">
@@ -2208,10 +2207,10 @@
       <c r="H29" t="s">
         <v>39</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J29" s="3" t="s">
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" t="s">
         <v>41</v>
       </c>
       <c r="K29" t="s">
@@ -2244,10 +2243,10 @@
       <c r="H30" t="s">
         <v>39</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J30" s="3" t="s">
+      <c r="I30" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" t="s">
         <v>41</v>
       </c>
       <c r="K30" t="s">
@@ -2280,10 +2279,10 @@
       <c r="H31" t="s">
         <v>39</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J31" s="3" t="s">
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
+      <c r="J31" t="s">
         <v>41</v>
       </c>
       <c r="K31" t="s">
@@ -2316,10 +2315,10 @@
       <c r="H32" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J32" s="3" t="s">
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" t="s">
         <v>41</v>
       </c>
       <c r="K32" t="s">
@@ -2352,10 +2351,10 @@
       <c r="H33" t="s">
         <v>39</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J33" s="3" t="s">
+      <c r="I33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" t="s">
         <v>41</v>
       </c>
       <c r="K33" t="s">
@@ -2388,10 +2387,10 @@
       <c r="H34" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J34" s="3" t="s">
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" t="s">
         <v>41</v>
       </c>
       <c r="K34" t="s">
@@ -2424,10 +2423,10 @@
       <c r="H35" t="s">
         <v>39</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J35" s="3" t="s">
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" t="s">
         <v>41</v>
       </c>
       <c r="K35" t="s">
@@ -2460,10 +2459,10 @@
       <c r="H36" t="s">
         <v>39</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J36" s="3" t="s">
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" t="s">
         <v>41</v>
       </c>
       <c r="K36" t="s">
@@ -2496,10 +2495,10 @@
       <c r="H37" t="s">
         <v>39</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J37" s="3" t="s">
+      <c r="I37" t="s">
+        <v>37</v>
+      </c>
+      <c r="J37" t="s">
         <v>41</v>
       </c>
       <c r="K37" t="s">
@@ -2532,10 +2531,10 @@
       <c r="H38" t="s">
         <v>39</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J38" s="3" t="s">
+      <c r="I38" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" t="s">
         <v>41</v>
       </c>
       <c r="K38" t="s">
@@ -2568,10 +2567,10 @@
       <c r="H39" t="s">
         <v>39</v>
       </c>
-      <c r="I39" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J39" s="3" t="s">
+      <c r="I39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" t="s">
         <v>41</v>
       </c>
       <c r="K39" t="s">
@@ -2604,10 +2603,10 @@
       <c r="H40" t="s">
         <v>39</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J40" s="3" t="s">
+      <c r="I40" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" t="s">
         <v>41</v>
       </c>
       <c r="K40" t="s">
@@ -2640,10 +2639,10 @@
       <c r="H41" t="s">
         <v>39</v>
       </c>
-      <c r="I41" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J41" s="3" t="s">
+      <c r="I41" t="s">
+        <v>37</v>
+      </c>
+      <c r="J41" t="s">
         <v>41</v>
       </c>
       <c r="K41" t="s">
@@ -2676,10 +2675,10 @@
       <c r="H42" t="s">
         <v>39</v>
       </c>
-      <c r="I42" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J42" s="3" t="s">
+      <c r="I42" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" t="s">
         <v>41</v>
       </c>
       <c r="K42" t="s">
@@ -2712,10 +2711,10 @@
       <c r="H43" t="s">
         <v>39</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J43" s="3" t="s">
+      <c r="I43" t="s">
+        <v>37</v>
+      </c>
+      <c r="J43" t="s">
         <v>41</v>
       </c>
       <c r="K43" t="s">
@@ -2748,10 +2747,10 @@
       <c r="H44" t="s">
         <v>39</v>
       </c>
-      <c r="I44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J44" s="3" t="s">
+      <c r="I44" t="s">
+        <v>37</v>
+      </c>
+      <c r="J44" t="s">
         <v>41</v>
       </c>
       <c r="K44" t="s">
@@ -2784,10 +2783,10 @@
       <c r="H45" t="s">
         <v>39</v>
       </c>
-      <c r="I45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J45" s="3" t="s">
+      <c r="I45" t="s">
+        <v>37</v>
+      </c>
+      <c r="J45" t="s">
         <v>41</v>
       </c>
       <c r="K45" t="s">
@@ -2820,10 +2819,10 @@
       <c r="H46" t="s">
         <v>39</v>
       </c>
-      <c r="I46" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J46" s="3" t="s">
+      <c r="I46" t="s">
+        <v>37</v>
+      </c>
+      <c r="J46" t="s">
         <v>41</v>
       </c>
       <c r="K46" t="s">
@@ -2844,7 +2843,7 @@
         <v>202</v>
       </c>
       <c r="D47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s">
@@ -2856,10 +2855,10 @@
       <c r="H47" t="s">
         <v>39</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J47" s="3" t="s">
+      <c r="I47" t="s">
+        <v>37</v>
+      </c>
+      <c r="J47" t="s">
         <v>41</v>
       </c>
       <c r="K47" t="s">
@@ -2891,8 +2890,8 @@
       <c r="H48" t="s">
         <v>39</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>235</v>
+      <c r="I48" t="s">
+        <v>236</v>
       </c>
       <c r="J48" t="s">
         <v>45</v>
@@ -2926,7 +2925,7 @@
       <c r="H49" t="s">
         <v>39</v>
       </c>
-      <c r="I49" s="3" t="s">
+      <c r="I49" t="s">
         <v>37</v>
       </c>
       <c r="J49" t="s">

</xml_diff>

<commit_message>
Added additional notes to some variables
</commit_message>
<xml_diff>
--- a/ges_health_study_app/dictionary_english.xlsx
+++ b/ges_health_study_app/dictionary_english.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1157A71-72DE-9740-AC2A-2B372274A715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2EECC5-CDE4-BB41-B41A-02DDF6B0ED64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{FBC012AF-A400-554A-B28E-7E1CB6FB8950}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="243">
   <si>
     <t>pct_nhb</t>
   </si>
@@ -134,12 +134,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>Housing built before 1980 puts children at risk of lead exposure.</t>
-  </si>
-  <si>
-    <t>This data set considers only noise from transportation sources.</t>
-  </si>
-  <si>
     <t>Unemployment estimates consider the civilian population between the ages of 18 and 64.</t>
   </si>
   <si>
@@ -372,9 +366,6 @@
   </si>
   <si>
     <t>CO</t>
-  </si>
-  <si>
-    <t>Estimates at the neighborhood level are based on inverse-distance weighting of average data at EPA AQS monitoring sites</t>
   </si>
   <si>
     <t>ppb</t>
@@ -575,69 +566,6 @@
     <t>Smoking</t>
   </si>
   <si>
-    <t>Depression among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Stroke among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Coronary heart disease among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Sleeping less than 7 hours among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Cancer (excluding skin cancer) among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Mental health not good for &gt;=14 days among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Chronic obstructive pulmonary disease among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Current asthma among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Older adult men aged &gt;=65 years who are up to date on a core set of clinical preventive services: Flu shot past year, PPV shot ever, Colorectal cancer screening (percent)</t>
-  </si>
-  <si>
-    <t>Visits to doctor for routine checkup within the past year among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Diagnosed diabetes among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Current smoking among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Fair or poor self-rated health status among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>High cholesterol among adults aged &gt;=18 years who have been screened in the past 5 years (percent)</t>
-  </si>
-  <si>
-    <t>Visits to dentist or dental clinic among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Obesity among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>No leisure-time physical activity among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Cervical cancer screening among adult women aged 21-65 years (percent)</t>
-  </si>
-  <si>
-    <t>High blood pressure among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>Older adult women aged &gt;=65 years who are up to date on a core set of clinical preventive services: Flu shot past year, PPV shot ever, Colorectal cancer screening, and Mammogram past 2 years (percent)</t>
-  </si>
-  <si>
-    <t>Fecal occult blood test, sigmoidoscopy, or colonoscopy among adults aged 50-75 years (percent)</t>
-  </si>
-  <si>
     <t>Fair or Poor Health</t>
   </si>
   <si>
@@ -668,72 +596,6 @@
     <t>Chronic Kidney Disease</t>
   </si>
   <si>
-    <t>depression among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>stroke among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>coronary heart disease among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>sleeping less than 7 hours among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>cancer (excluding skin cancer) among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>mental health not good for &gt;=14 days among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>chronic obstructive pulmonary disease among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>current asthma among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>older adult men aged &gt;=65 years who are up to date on a core set of clinical preventive services: flu shot past year, ppv shot ever, colorectal cancer screening (percent)</t>
-  </si>
-  <si>
-    <t>visits to doctor for routine checkup within the past year among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>diagnosed diabetes among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>current smoking among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>fair or poor self-rated health status among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>high cholesterol among adults aged &gt;=18 years who have been screened in the past 5 years (percent)</t>
-  </si>
-  <si>
-    <t>visits to dentist or dental clinic among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>obesity among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>no leisure-time physical activity among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>cervical cancer screening among adult women aged 21-65 years (percent)</t>
-  </si>
-  <si>
-    <t>high blood pressure among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
-    <t>older adult women aged &gt;=65 years who are up to date on a core set of clinical preventive services: flu shot past year, ppv shot ever, colorectal cancer screening, and mammogram past 2 years (percent)</t>
-  </si>
-  <si>
-    <t>fecal occult blood test, sigmoidoscopy, or colonoscopy among adults aged 50-75 years (percent)</t>
-  </si>
-  <si>
-    <t>chronic kidney disease among adults aged &gt;=18 years (percent)</t>
-  </si>
-  <si>
     <t>CDC PLACES (2023 Release)</t>
   </si>
   <si>
@@ -764,13 +626,166 @@
     <t>lbw_pct</t>
   </si>
   <si>
-    <t xml:space="preserve">Chronic kidney disease among adults aged &gt;=18 years </t>
-  </si>
-  <si>
     <t>Cases per 10,000</t>
   </si>
   <si>
     <t>years</t>
+  </si>
+  <si>
+    <t>Supplemental Nutrition Assistance Program (SNAP) benefits help low-income families supplement their grocery budget.</t>
+  </si>
+  <si>
+    <t>Numbers above 1 indicate more alcohol retail outlets than food stores in a neighborhood.</t>
+  </si>
+  <si>
+    <t>Numbers above 1 indicate more cannabis cultivation sites than food stores in a neighborhood.</t>
+  </si>
+  <si>
+    <t>Estimates at the neighborhood level are based on inverse-distance weighting of average data at EPA AQS monitoring sites.</t>
+  </si>
+  <si>
+    <t>Housing built before 1980 puts children at higher risk of lead exposure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of chronic kidney disease among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of depression among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of stroke among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of coronary heart disease among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of sleeping less than 7 hours among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of cancer (excluding skin cancer) among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of mental health not good for &gt;=14 days among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of chronic obstructive pulmonary disease among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of current asthma among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of older adult men aged &gt;=65 years who are up to date on a core set of clinical preventive services: flu shot past year, ppv shot ever, colorectal cancer screening </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of visits to doctor for routine checkup within the past year among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of diagnosed diabetes among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of current smoking among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of fair or poor self-rated health status among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of high cholesterol among adults aged &gt;=18 years who have been screened in the past 5 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of visits to dentist or dental clinic among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of obesity among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of no leisure-time physical activity among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of cervical cancer screening among adult women aged 21-65 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of high blood pressure among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of older adult women aged &gt;=65 years who are up to date on a core set of clinical preventive services: flu shot past year, ppv shot ever, colorectal cancer screening, and mammogram past 2 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevalence of fecal occult blood test, sigmoidoscopy, or colonoscopy among adults aged 50-75 years </t>
+  </si>
+  <si>
+    <t>Higher scores indicate neighborhoods with better tree coverage to meet health and climate change needs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This data set considers only noise from transportation sources. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of depression among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of stroke among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of coronary heart disease among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of sleeping less than 7 hours among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of cancer (excluding skin cancer) among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of mental health not good for &gt;=14 days among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of chronic obstructive pulmonary disease among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of current asthma among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of older adult men aged &gt;=65 years who are up to date on a core set of clinical preventive services: flu shot past year, ppv shot ever, colorectal cancer screening </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of visits to doctor for routine checkup within the past year among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of diagnosed diabetes among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of current smoking among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of fair or poor self-rated health status among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of high cholesterol among adults aged &gt;=18 years who have been screened in the past 5 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of visits to dentist or dental clinic among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of obesity among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of no leisure-time physical activity among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of cervical cancer screening among adult women aged 21-65 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of high blood pressure among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of older adult women aged &gt;=65 years who are up to date on a core set of clinical preventive services: flu shot past year, ppv shot ever, colorectal cancer screening, and mammogram past 2 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of fecal occult blood test, sigmoidoscopy, or colonoscopy among adults aged 50-75 years </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevalence of chronic kidney disease among adults aged &gt;=18 years </t>
+  </si>
+  <si>
+    <t>Higher numbers indicate hotter street temperatures.</t>
   </si>
 </sst>
 </file>
@@ -819,12 +834,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEABDE7F-51DA-E349-ABBB-2A88FDA51C20}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1170,22 +1186,22 @@
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="50.1640625" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="87.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
@@ -1197,30 +1213,30 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
       <c r="K1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -1232,30 +1248,30 @@
         <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1267,30 +1283,30 @@
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -1302,33 +1318,33 @@
         <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
@@ -1337,33 +1353,36 @@
         <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" t="s">
-        <v>89</v>
+      <c r="E6" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -1372,30 +1391,30 @@
         <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -1407,33 +1426,33 @@
         <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
@@ -1442,36 +1461,36 @@
         <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -1480,30 +1499,30 @@
         <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -1515,33 +1534,33 @@
         <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" t="s">
         <v>93</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" t="s">
-        <v>95</v>
       </c>
       <c r="F11" t="s">
         <v>26</v>
@@ -1550,62 +1569,65 @@
         <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" t="s">
-        <v>62</v>
-      </c>
       <c r="J12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
@@ -1613,40 +1635,43 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
+      <c r="E13" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="F13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G13" t="s">
         <v>25</v>
       </c>
       <c r="H13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
@@ -1655,59 +1680,62 @@
         <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F15" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" t="s">
         <v>81</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" t="s">
-        <v>75</v>
-      </c>
-      <c r="J15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L15" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -1719,7 +1747,7 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>219</v>
       </c>
       <c r="F16" t="s">
         <v>29</v>
@@ -1728,24 +1756,24 @@
         <v>25</v>
       </c>
       <c r="H16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>10</v>
@@ -1756,6 +1784,9 @@
       <c r="D17" t="s">
         <v>22</v>
       </c>
+      <c r="E17" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="F17" t="s">
         <v>28</v>
       </c>
@@ -1763,36 +1794,36 @@
         <v>25</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
       </c>
-      <c r="E18" t="s">
-        <v>32</v>
+      <c r="E18" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="F18" t="s">
         <v>26</v>
@@ -1801,36 +1832,36 @@
         <v>25</v>
       </c>
       <c r="H18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
@@ -1839,36 +1870,36 @@
         <v>25</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I19" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -1877,36 +1908,36 @@
         <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I20" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
@@ -1915,36 +1946,36 @@
         <v>25</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E22" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
@@ -1953,36 +1984,36 @@
         <v>25</v>
       </c>
       <c r="H22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F23" t="s">
         <v>24</v>
@@ -1991,36 +2022,36 @@
         <v>25</v>
       </c>
       <c r="H23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="F24" t="s">
         <v>24</v>
@@ -2029,916 +2060,918 @@
         <v>25</v>
       </c>
       <c r="H24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="J25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25" t="s">
+        <v>190</v>
+      </c>
+      <c r="L25" t="s">
         <v>134</v>
-      </c>
-      <c r="G25" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25" t="s">
-        <v>135</v>
-      </c>
-      <c r="J25" t="s">
-        <v>45</v>
-      </c>
-      <c r="K25" t="s">
-        <v>237</v>
-      </c>
-      <c r="L25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G26" t="s">
         <v>25</v>
       </c>
       <c r="H26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L26" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D27" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G27" t="s">
         <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L27" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D28" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G28" t="s">
         <v>25</v>
       </c>
       <c r="H28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L28" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D29" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G29" t="s">
         <v>25</v>
       </c>
       <c r="H29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L29" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D30" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G30" t="s">
         <v>25</v>
       </c>
       <c r="H30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L30" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s">
+        <v>179</v>
+      </c>
+      <c r="G31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31" t="s">
         <v>225</v>
-      </c>
-      <c r="G31" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" t="s">
-        <v>39</v>
-      </c>
-      <c r="I31" t="s">
-        <v>37</v>
-      </c>
-      <c r="J31" t="s">
-        <v>41</v>
-      </c>
-      <c r="K31" t="s">
-        <v>41</v>
-      </c>
-      <c r="L31" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D32" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G32" t="s">
         <v>25</v>
       </c>
       <c r="H32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L32" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D33" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G33" t="s">
         <v>25</v>
       </c>
       <c r="H33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L33" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G34" t="s">
         <v>25</v>
       </c>
       <c r="H34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L34" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G35" t="s">
         <v>25</v>
       </c>
       <c r="H35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L35" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D36" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G36" t="s">
         <v>25</v>
       </c>
       <c r="H36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L36" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D37" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G37" t="s">
         <v>25</v>
       </c>
       <c r="H37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L37" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="D38" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G38" t="s">
         <v>25</v>
       </c>
       <c r="H38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L38" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="D39" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G39" t="s">
         <v>25</v>
       </c>
       <c r="H39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L39" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="D40" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G40" t="s">
         <v>25</v>
       </c>
       <c r="H40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L40" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="D41" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G41" t="s">
         <v>25</v>
       </c>
       <c r="H41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L41" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B42" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D42" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G42" t="s">
         <v>25</v>
       </c>
       <c r="H42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I42" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L42" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="D43" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G43" t="s">
         <v>25</v>
       </c>
       <c r="H43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L43" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D44" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G44" t="s">
         <v>25</v>
       </c>
       <c r="H44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L44" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B45" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="D45" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G45" t="s">
         <v>25</v>
       </c>
       <c r="H45" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L45" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="D46" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G46" t="s">
         <v>25</v>
       </c>
       <c r="H46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L46" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="D47" t="s">
-        <v>235</v>
+        <v>196</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="G47" t="s">
         <v>25</v>
       </c>
       <c r="H47" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L47" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B48" t="s">
-        <v>226</v>
+        <v>180</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>227</v>
+        <v>181</v>
       </c>
       <c r="D48" t="s">
-        <v>232</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="E48" s="2"/>
       <c r="F48" t="s">
-        <v>228</v>
+        <v>182</v>
       </c>
       <c r="G48" t="s">
         <v>25</v>
       </c>
       <c r="H48" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I48" t="s">
-        <v>236</v>
+        <v>189</v>
       </c>
       <c r="J48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K48" t="s">
-        <v>233</v>
+        <v>187</v>
       </c>
       <c r="L48" t="s">
-        <v>232</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B49" t="s">
-        <v>234</v>
+        <v>188</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>229</v>
+        <v>183</v>
       </c>
       <c r="D49" t="s">
-        <v>230</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E49" s="2"/>
       <c r="F49" t="s">
-        <v>228</v>
+        <v>182</v>
       </c>
       <c r="G49" t="s">
         <v>25</v>
       </c>
       <c r="H49" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I49" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L49" t="s">
-        <v>231</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
miinor corrections to the alt text
</commit_message>
<xml_diff>
--- a/ges_health_study_app/dictionary_english.xlsx
+++ b/ges_health_study_app/dictionary_english.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2EECC5-CDE4-BB41-B41A-02DDF6B0ED64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405FA554-98E6-284C-B224-70C5E732D926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{FBC012AF-A400-554A-B28E-7E1CB6FB8950}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FBC012AF-A400-554A-B28E-7E1CB6FB8950}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -281,9 +281,6 @@
     <t>Average percentile ranking of surface temperatures for streets in the neighborhood</t>
   </si>
   <si>
-    <t>average percentile ranking of surface temperatures for streets in the neighborhood</t>
-  </si>
-  <si>
     <t>short_var_name</t>
   </si>
   <si>
@@ -390,24 +387,6 @@
   </si>
   <si>
     <t>Average ambient CO at the neighborhood level (2017-2021)</t>
-  </si>
-  <si>
-    <t>average ambient PM2.5 at the neighborhood level (2017-2021)</t>
-  </si>
-  <si>
-    <t>average ambient O3 at the neighborhood level (2017-2021)</t>
-  </si>
-  <si>
-    <t>average ambient PM10 at the neighborhood level (2017-2021)</t>
-  </si>
-  <si>
-    <t>average ambient NO2 at the neighborhood level (2017-2021)</t>
-  </si>
-  <si>
-    <t>average ambient SO2 at the neighborhood level (2017-2021)</t>
-  </si>
-  <si>
-    <t>average ambient CO at the neighborhood level (2017-2021)</t>
   </si>
   <si>
     <t>Colorado Department of Revenue, City and County of Denver</t>
@@ -786,6 +765,27 @@
   </si>
   <si>
     <t>Higher numbers indicate hotter street temperatures.</t>
+  </si>
+  <si>
+    <t>average ambient PM2.5 (2017-2021)</t>
+  </si>
+  <si>
+    <t>average ambient O3 (2017-2021)</t>
+  </si>
+  <si>
+    <t>average ambient PM10 (2017-2021)</t>
+  </si>
+  <si>
+    <t>average ambient NO2 (2017-2021)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average percentile ranking of street surface temperatures </t>
+  </si>
+  <si>
+    <t>average ambient SO2 (2017-2021)</t>
+  </si>
+  <si>
+    <t>average ambient CO (2017-2021)</t>
   </si>
 </sst>
 </file>
@@ -834,13 +834,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,7 +1177,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1192,16 +1191,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
       </c>
       <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
         <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
       </c>
       <c r="E1" t="s">
         <v>31</v>
@@ -1225,12 +1224,12 @@
         <v>41</v>
       </c>
       <c r="L1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1265,7 +1264,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -1300,7 +1299,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1335,7 +1334,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -1370,19 +1369,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" t="s">
         <v>86</v>
       </c>
-      <c r="D6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>191</v>
+      <c r="E6" t="s">
+        <v>184</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -1403,12 +1402,12 @@
         <v>39</v>
       </c>
       <c r="L6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
@@ -1443,7 +1442,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
@@ -1478,7 +1477,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -1511,12 +1510,12 @@
         <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -1546,21 +1545,21 @@
         <v>39</v>
       </c>
       <c r="L10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" t="s">
         <v>92</v>
-      </c>
-      <c r="D11" t="s">
-        <v>93</v>
       </c>
       <c r="F11" t="s">
         <v>26</v>
@@ -1581,12 +1580,12 @@
         <v>39</v>
       </c>
       <c r="L11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>57</v>
@@ -1597,11 +1596,11 @@
       <c r="D12" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>192</v>
+      <c r="E12" t="s">
+        <v>185</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
@@ -1624,7 +1623,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>56</v>
@@ -1635,11 +1634,11 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>193</v>
+      <c r="E13" t="s">
+        <v>186</v>
       </c>
       <c r="F13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G13" t="s">
         <v>25</v>
@@ -1662,7 +1661,7 @@
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>75</v>
@@ -1697,7 +1696,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>77</v>
@@ -1708,8 +1707,8 @@
       <c r="D15" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>242</v>
+      <c r="E15" t="s">
+        <v>235</v>
       </c>
       <c r="F15" t="s">
         <v>79</v>
@@ -1730,12 +1729,12 @@
         <v>43</v>
       </c>
       <c r="L15" t="s">
-        <v>81</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -1747,7 +1746,7 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F16" t="s">
         <v>29</v>
@@ -1773,7 +1772,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>10</v>
@@ -1784,8 +1783,8 @@
       <c r="D17" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>218</v>
+      <c r="E17" t="s">
+        <v>211</v>
       </c>
       <c r="F17" t="s">
         <v>28</v>
@@ -1811,7 +1810,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>30</v>
@@ -1822,8 +1821,8 @@
       <c r="D18" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>195</v>
+      <c r="E18" t="s">
+        <v>188</v>
       </c>
       <c r="F18" t="s">
         <v>26</v>
@@ -1849,19 +1848,19 @@
     </row>
     <row r="19" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
@@ -1873,7 +1872,7 @@
         <v>37</v>
       </c>
       <c r="I19" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="J19" t="s">
         <v>43</v>
@@ -1882,24 +1881,24 @@
         <v>42</v>
       </c>
       <c r="L19" t="s">
-        <v>118</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -1911,33 +1910,33 @@
         <v>37</v>
       </c>
       <c r="I20" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="J20" t="s">
         <v>43</v>
       </c>
       <c r="K20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L20" t="s">
-        <v>119</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
@@ -1949,7 +1948,7 @@
         <v>37</v>
       </c>
       <c r="I21" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="J21" t="s">
         <v>43</v>
@@ -1958,24 +1957,24 @@
         <v>42</v>
       </c>
       <c r="L21" t="s">
-        <v>120</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
@@ -1987,33 +1986,33 @@
         <v>37</v>
       </c>
       <c r="I22" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="J22" t="s">
         <v>43</v>
       </c>
       <c r="K22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L22" t="s">
-        <v>121</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E23" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F23" t="s">
         <v>24</v>
@@ -2025,33 +2024,33 @@
         <v>37</v>
       </c>
       <c r="I23" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="J23" t="s">
         <v>43</v>
       </c>
       <c r="K23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L23" t="s">
-        <v>122</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E24" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F24" t="s">
         <v>24</v>
@@ -2063,33 +2062,33 @@
         <v>37</v>
       </c>
       <c r="I24" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="J24" t="s">
         <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L24" t="s">
-        <v>123</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F25" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G25" t="s">
         <v>25</v>
@@ -2098,34 +2097,34 @@
         <v>37</v>
       </c>
       <c r="I25" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J25" t="s">
         <v>43</v>
       </c>
       <c r="K25" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="L25" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" t="s">
         <v>128</v>
       </c>
-      <c r="B26" t="s">
-        <v>135</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D26" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G26" t="s">
         <v>25</v>
@@ -2143,25 +2142,25 @@
         <v>39</v>
       </c>
       <c r="L26" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D27" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G27" t="s">
         <v>25</v>
@@ -2179,25 +2178,25 @@
         <v>39</v>
       </c>
       <c r="L27" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G28" t="s">
         <v>25</v>
@@ -2215,25 +2214,25 @@
         <v>39</v>
       </c>
       <c r="L28" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D29" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G29" t="s">
         <v>25</v>
@@ -2251,25 +2250,25 @@
         <v>39</v>
       </c>
       <c r="L29" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D30" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G30" t="s">
         <v>25</v>
@@ -2287,25 +2286,25 @@
         <v>39</v>
       </c>
       <c r="L30" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D31" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G31" t="s">
         <v>25</v>
@@ -2323,25 +2322,25 @@
         <v>39</v>
       </c>
       <c r="L31" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D32" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G32" t="s">
         <v>25</v>
@@ -2359,25 +2358,25 @@
         <v>39</v>
       </c>
       <c r="L32" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D33" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G33" t="s">
         <v>25</v>
@@ -2395,25 +2394,25 @@
         <v>39</v>
       </c>
       <c r="L33" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D34" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G34" t="s">
         <v>25</v>
@@ -2431,25 +2430,25 @@
         <v>39</v>
       </c>
       <c r="L34" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D35" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G35" t="s">
         <v>25</v>
@@ -2467,25 +2466,25 @@
         <v>39</v>
       </c>
       <c r="L35" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D36" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G36" t="s">
         <v>25</v>
@@ -2503,25 +2502,25 @@
         <v>39</v>
       </c>
       <c r="L36" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D37" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G37" t="s">
         <v>25</v>
@@ -2539,25 +2538,25 @@
         <v>39</v>
       </c>
       <c r="L37" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G38" t="s">
         <v>25</v>
@@ -2575,25 +2574,25 @@
         <v>39</v>
       </c>
       <c r="L38" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D39" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G39" t="s">
         <v>25</v>
@@ -2611,25 +2610,25 @@
         <v>39</v>
       </c>
       <c r="L39" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B40" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D40" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G40" t="s">
         <v>25</v>
@@ -2647,25 +2646,25 @@
         <v>39</v>
       </c>
       <c r="L40" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D41" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G41" t="s">
         <v>25</v>
@@ -2683,25 +2682,25 @@
         <v>39</v>
       </c>
       <c r="L41" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D42" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G42" t="s">
         <v>25</v>
@@ -2719,25 +2718,25 @@
         <v>39</v>
       </c>
       <c r="L42" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G43" t="s">
         <v>25</v>
@@ -2755,25 +2754,25 @@
         <v>39</v>
       </c>
       <c r="L43" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G44" t="s">
         <v>25</v>
@@ -2791,25 +2790,25 @@
         <v>39</v>
       </c>
       <c r="L44" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B45" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D45" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G45" t="s">
         <v>25</v>
@@ -2827,25 +2826,25 @@
         <v>39</v>
       </c>
       <c r="L45" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G46" t="s">
         <v>25</v>
@@ -2863,25 +2862,25 @@
         <v>39</v>
       </c>
       <c r="L46" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G47" t="s">
         <v>25</v>
@@ -2899,61 +2898,61 @@
         <v>39</v>
       </c>
       <c r="L47" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D48" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s">
+        <v>175</v>
+      </c>
+      <c r="G48" t="s">
+        <v>25</v>
+      </c>
+      <c r="H48" t="s">
+        <v>37</v>
+      </c>
+      <c r="I48" t="s">
         <v>182</v>
-      </c>
-      <c r="G48" t="s">
-        <v>25</v>
-      </c>
-      <c r="H48" t="s">
-        <v>37</v>
-      </c>
-      <c r="I48" t="s">
-        <v>189</v>
       </c>
       <c r="J48" t="s">
         <v>43</v>
       </c>
       <c r="K48" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="L48" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D49" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G49" t="s">
         <v>25</v>
@@ -2971,7 +2970,7 @@
         <v>39</v>
       </c>
       <c r="L49" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating with Spanish language translation
</commit_message>
<xml_diff>
--- a/ges_health_study_app/dictionary_english.xlsx
+++ b/ges_health_study_app/dictionary_english.xlsx
@@ -2976,4 +2976,273 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010004A00BE2561B93438AA360303F4E6ECF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="16c84a0256324123b976d8a27aa8ee24">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c3b28d1-dd5b-4818-90bf-d163a72c8f0a" xmlns:ns3="a37677e5-1b95-4b15-ad17-c2245905d011" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad974ad6d367d52b8cbe38bd7ba58e6d" ns2:_="" ns3:_="">
+    <xsd:import namespace="8c3b28d1-dd5b-4818-90bf-d163a72c8f0a"/>
+    <xsd:import namespace="a37677e5-1b95-4b15-ad17-c2245905d011"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8c3b28d1-dd5b-4818-90bf-d163a72c8f0a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="576e6ad8-52fe-412f-a0b9-03ea580b6293" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a37677e5-1b95-4b15-ad17-c2245905d011" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{7e59bb6d-7fc5-4261-a11f-14ab589c08fc}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="a37677e5-1b95-4b15-ad17-c2245905d011">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a37677e5-1b95-4b15-ad17-c2245905d011" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8c3b28d1-dd5b-4818-90bf-d163a72c8f0a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D90268-E8C1-455D-AAB6-78B7985F3EA3}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A383C752-A17F-42FC-AE6E-92B0304EE37D}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68CED3EF-3E9C-434C-A0BD-96F22D288659}"/>
 </file>
</xml_diff>